<commit_message>
edits to ch6 and ch9
</commit_message>
<xml_diff>
--- a/tables/ch6/cnt-device-parameters.xlsx
+++ b/tables/ch6/cnt-device-parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vuw-my.sharepoint.com/personal/treachne_staff_vuw_ac_nz/Documents/Ned_Natalie_PhD/PhD-thesis/phd-thesis/tables/ch5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vuw-my.sharepoint.com/personal/treachne_staff_vuw_ac_nz/Documents/Ned_Natalie_PhD/PhD-thesis/phd-thesis/tables/ch6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="676" documentId="11_F25DC773A252ABDACC1048F3819E6E4C5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08300F99-4744-44E2-AE9D-17965DC1B414}"/>
+  <xr:revisionPtr revIDLastSave="678" documentId="11_F25DC773A252ABDACC1048F3819E6E4C5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E359162D-3FA7-4590-8D83-F9179FF8187B}"/>
   <bookViews>
-    <workbookView xWindow="-540" yWindow="2025" windowWidth="13155" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2760" yWindow="1575" windowWidth="12720" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -453,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>